<commit_message>
sigmoid iteration, 0.54 r-squared
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -456,46 +456,46 @@
         <v>65</v>
       </c>
       <c r="B4" t="n">
-        <v>2657.84</v>
+        <v>2287.81</v>
       </c>
       <c r="C4" t="n">
-        <v>3028.87</v>
+        <v>2731.01</v>
       </c>
       <c r="D4" t="n">
-        <v>3399.9</v>
+        <v>4300.83</v>
       </c>
       <c r="E4" t="n">
-        <v>3770.93</v>
+        <v>4977.32</v>
       </c>
       <c r="F4" t="n">
-        <v>4141.96</v>
+        <v>4791.22</v>
       </c>
       <c r="G4" t="n">
-        <v>4512.99</v>
+        <v>4332.28</v>
       </c>
       <c r="H4" t="n">
-        <v>4884.01</v>
+        <v>3803.81</v>
       </c>
       <c r="I4" t="n">
-        <v>5255.04</v>
+        <v>3381.93</v>
       </c>
       <c r="J4" t="n">
-        <v>5626.07</v>
+        <v>3137.76</v>
       </c>
       <c r="K4" t="n">
-        <v>5997.1</v>
+        <v>3023.37</v>
       </c>
       <c r="L4" t="n">
-        <v>6368.13</v>
+        <v>2975.24</v>
       </c>
       <c r="M4" t="n">
-        <v>6739.16</v>
+        <v>2955.91</v>
       </c>
       <c r="N4" t="n">
-        <v>7110.19</v>
+        <v>2948.3</v>
       </c>
       <c r="O4" t="n">
-        <v>7481.21</v>
+        <v>2945.33</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -503,46 +503,46 @@
         <v>70</v>
       </c>
       <c r="B5" t="n">
-        <v>2939.87</v>
+        <v>2532.19</v>
       </c>
       <c r="C5" t="n">
-        <v>3310.9</v>
+        <v>2789.23</v>
       </c>
       <c r="D5" t="n">
-        <v>3681.93</v>
+        <v>4172.95</v>
       </c>
       <c r="E5" t="n">
-        <v>4052.96</v>
+        <v>4809.86</v>
       </c>
       <c r="F5" t="n">
-        <v>4423.99</v>
+        <v>4552.18</v>
       </c>
       <c r="G5" t="n">
-        <v>4795.01</v>
+        <v>4048.08</v>
       </c>
       <c r="H5" t="n">
-        <v>5166.04</v>
+        <v>3572.22</v>
       </c>
       <c r="I5" t="n">
-        <v>5537.07</v>
+        <v>3265.87</v>
       </c>
       <c r="J5" t="n">
-        <v>5908.1</v>
+        <v>3113.5</v>
       </c>
       <c r="K5" t="n">
-        <v>6279.13</v>
+        <v>3047.56</v>
       </c>
       <c r="L5" t="n">
-        <v>6650.16</v>
+        <v>3020.78</v>
       </c>
       <c r="M5" t="n">
-        <v>7021.19</v>
+        <v>3010.18</v>
       </c>
       <c r="N5" t="n">
-        <v>7392.21</v>
+        <v>3006.03</v>
       </c>
       <c r="O5" t="n">
-        <v>7763.24</v>
+        <v>3004.41</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -550,46 +550,46 @@
         <v>75</v>
       </c>
       <c r="B6" t="n">
-        <v>3221.9</v>
+        <v>2893.4</v>
       </c>
       <c r="C6" t="n">
-        <v>3592.93</v>
+        <v>2987.66</v>
       </c>
       <c r="D6" t="n">
-        <v>3963.96</v>
+        <v>4142.43</v>
       </c>
       <c r="E6" t="n">
-        <v>4334.99</v>
+        <v>4700.02</v>
       </c>
       <c r="F6" t="n">
-        <v>4706.01</v>
+        <v>4367.59</v>
       </c>
       <c r="G6" t="n">
-        <v>5077.04</v>
+        <v>3881.49</v>
       </c>
       <c r="H6" t="n">
-        <v>5448.07</v>
+        <v>3515.53</v>
       </c>
       <c r="I6" t="n">
-        <v>5819.1</v>
+        <v>3317.8</v>
       </c>
       <c r="J6" t="n">
-        <v>6190.13</v>
+        <v>3228.8</v>
       </c>
       <c r="K6" t="n">
-        <v>6561.16</v>
+        <v>3192.02</v>
       </c>
       <c r="L6" t="n">
-        <v>6932.19</v>
+        <v>3177.38</v>
       </c>
       <c r="M6" t="n">
-        <v>7303.21</v>
+        <v>3171.62</v>
       </c>
       <c r="N6" t="n">
-        <v>7674.24</v>
+        <v>3169.38</v>
       </c>
       <c r="O6" t="n">
-        <v>8045.27</v>
+        <v>3168.5</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -597,46 +597,46 @@
         <v>80</v>
       </c>
       <c r="B7" t="n">
-        <v>3503.93</v>
+        <v>3369.4</v>
       </c>
       <c r="C7" t="n">
-        <v>3874.96</v>
+        <v>3339.81</v>
       </c>
       <c r="D7" t="n">
-        <v>4245.99</v>
+        <v>4237.68</v>
       </c>
       <c r="E7" t="n">
-        <v>4617.01</v>
+        <v>4688.55</v>
       </c>
       <c r="F7" t="n">
-        <v>4988.04</v>
+        <v>4317.99</v>
       </c>
       <c r="G7" t="n">
-        <v>5359.07</v>
+        <v>3917.51</v>
       </c>
       <c r="H7" t="n">
-        <v>5730.1</v>
+        <v>3672.24</v>
       </c>
       <c r="I7" t="n">
-        <v>6101.13</v>
+        <v>3555.28</v>
       </c>
       <c r="J7" t="n">
-        <v>6472.16</v>
+        <v>3505.74</v>
       </c>
       <c r="K7" t="n">
-        <v>6843.19</v>
+        <v>3485.8</v>
       </c>
       <c r="L7" t="n">
-        <v>7214.21</v>
+        <v>3477.94</v>
       </c>
       <c r="M7" t="n">
-        <v>7585.24</v>
+        <v>3474.87</v>
       </c>
       <c r="N7" t="n">
-        <v>7956.27</v>
+        <v>3473.67</v>
       </c>
       <c r="O7" t="n">
-        <v>8327.299999999999</v>
+        <v>3473.2</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -644,46 +644,46 @@
         <v>85</v>
       </c>
       <c r="B8" t="n">
-        <v>3785.96</v>
+        <v>3941.11</v>
       </c>
       <c r="C8" t="n">
-        <v>4156.99</v>
+        <v>3821.79</v>
       </c>
       <c r="D8" t="n">
-        <v>4528.01</v>
+        <v>4467.43</v>
       </c>
       <c r="E8" t="n">
-        <v>4899.04</v>
+        <v>4828.62</v>
       </c>
       <c r="F8" t="n">
-        <v>5270.07</v>
+        <v>4482.67</v>
       </c>
       <c r="G8" t="n">
-        <v>5641.1</v>
+        <v>4195.31</v>
       </c>
       <c r="H8" t="n">
-        <v>6012.13</v>
+        <v>4046.04</v>
       </c>
       <c r="I8" t="n">
-        <v>6383.16</v>
+        <v>3980.57</v>
       </c>
       <c r="J8" t="n">
-        <v>6754.19</v>
+        <v>3953.84</v>
       </c>
       <c r="K8" t="n">
-        <v>7125.21</v>
+        <v>3943.25</v>
       </c>
       <c r="L8" t="n">
-        <v>7496.24</v>
+        <v>3939.1</v>
       </c>
       <c r="M8" t="n">
-        <v>7867.27</v>
+        <v>3937.48</v>
       </c>
       <c r="N8" t="n">
-        <v>8238.299999999999</v>
+        <v>3936.85</v>
       </c>
       <c r="O8" t="n">
-        <v>8609.33</v>
+        <v>3936.6</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -691,46 +691,46 @@
         <v>90</v>
       </c>
       <c r="B9" t="n">
-        <v>4067.99</v>
+        <v>4554.83</v>
       </c>
       <c r="C9" t="n">
-        <v>4439.01</v>
+        <v>4357.36</v>
       </c>
       <c r="D9" t="n">
-        <v>4810.04</v>
+        <v>4803.98</v>
       </c>
       <c r="E9" t="n">
-        <v>5181.07</v>
+        <v>5154.9</v>
       </c>
       <c r="F9" t="n">
-        <v>5552.1</v>
+        <v>4880.32</v>
       </c>
       <c r="G9" t="n">
-        <v>5923.13</v>
+        <v>4685.38</v>
       </c>
       <c r="H9" t="n">
-        <v>6294.16</v>
+        <v>4595</v>
       </c>
       <c r="I9" t="n">
-        <v>6665.19</v>
+        <v>4557.48</v>
       </c>
       <c r="J9" t="n">
-        <v>7036.21</v>
+        <v>4542.51</v>
       </c>
       <c r="K9" t="n">
-        <v>7407.24</v>
+        <v>4536.64</v>
       </c>
       <c r="L9" t="n">
-        <v>7778.27</v>
+        <v>4534.34</v>
       </c>
       <c r="M9" t="n">
-        <v>8149.3</v>
+        <v>4533.45</v>
       </c>
       <c r="N9" t="n">
-        <v>8520.33</v>
+        <v>4533.1</v>
       </c>
       <c r="O9" t="n">
-        <v>8891.360000000001</v>
+        <v>4532.96</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -738,46 +738,46 @@
         <v>95</v>
       </c>
       <c r="B10" t="n">
-        <v>4350.01</v>
+        <v>5111.12</v>
       </c>
       <c r="C10" t="n">
-        <v>4721.04</v>
+        <v>4831.74</v>
       </c>
       <c r="D10" t="n">
-        <v>5092.07</v>
+        <v>5180.17</v>
       </c>
       <c r="E10" t="n">
-        <v>5463.1</v>
+        <v>5636.09</v>
       </c>
       <c r="F10" t="n">
-        <v>5834.13</v>
+        <v>5443.29</v>
       </c>
       <c r="G10" t="n">
-        <v>6205.16</v>
+        <v>5294.61</v>
       </c>
       <c r="H10" t="n">
-        <v>6576.19</v>
+        <v>5226.58</v>
       </c>
       <c r="I10" t="n">
-        <v>6947.21</v>
+        <v>5198.58</v>
       </c>
       <c r="J10" t="n">
-        <v>7318.24</v>
+        <v>5187.47</v>
       </c>
       <c r="K10" t="n">
-        <v>7689.27</v>
+        <v>5183.11</v>
       </c>
       <c r="L10" t="n">
-        <v>8060.3</v>
+        <v>5181.41</v>
       </c>
       <c r="M10" t="n">
-        <v>8431.33</v>
+        <v>5180.74</v>
       </c>
       <c r="N10" t="n">
-        <v>8802.360000000001</v>
+        <v>5180.49</v>
       </c>
       <c r="O10" t="n">
-        <v>9173.389999999999</v>
+        <v>5180.39</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -785,46 +785,46 @@
         <v>100</v>
       </c>
       <c r="B11" t="n">
-        <v>4632.04</v>
+        <v>5496.16</v>
       </c>
       <c r="C11" t="n">
-        <v>5003.07</v>
+        <v>5147.12</v>
       </c>
       <c r="D11" t="n">
-        <v>5374.1</v>
+        <v>5511.97</v>
       </c>
       <c r="E11" t="n">
-        <v>5745.13</v>
+        <v>6171.5</v>
       </c>
       <c r="F11" t="n">
-        <v>6116.16</v>
+        <v>6056.89</v>
       </c>
       <c r="G11" t="n">
-        <v>6487.19</v>
+        <v>5907.82</v>
       </c>
       <c r="H11" t="n">
-        <v>6858.21</v>
+        <v>5828.78</v>
       </c>
       <c r="I11" t="n">
-        <v>7229.24</v>
+        <v>5794.08</v>
       </c>
       <c r="J11" t="n">
-        <v>7600.27</v>
+        <v>5779.92</v>
       </c>
       <c r="K11" t="n">
-        <v>7971.3</v>
+        <v>5774.3</v>
       </c>
       <c r="L11" t="n">
-        <v>8342.33</v>
+        <v>5772.1</v>
       </c>
       <c r="M11" t="n">
-        <v>8713.360000000001</v>
+        <v>5771.25</v>
       </c>
       <c r="N11" t="n">
-        <v>9084.389999999999</v>
+        <v>5770.91</v>
       </c>
       <c r="O11" t="n">
-        <v>9455.41</v>
+        <v>5770.78</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -832,46 +832,46 @@
         <v>105</v>
       </c>
       <c r="B12" t="n">
-        <v>4914.07</v>
+        <v>5646.88</v>
       </c>
       <c r="C12" t="n">
-        <v>5285.1</v>
+        <v>5276.9</v>
       </c>
       <c r="D12" t="n">
-        <v>5656.13</v>
+        <v>5734.17</v>
       </c>
       <c r="E12" t="n">
-        <v>6027.16</v>
+        <v>6647.43</v>
       </c>
       <c r="F12" t="n">
-        <v>6398.19</v>
+        <v>6624.01</v>
       </c>
       <c r="G12" t="n">
-        <v>6769.21</v>
+        <v>6445.17</v>
       </c>
       <c r="H12" t="n">
-        <v>7140.24</v>
+        <v>6324.83</v>
       </c>
       <c r="I12" t="n">
-        <v>7511.27</v>
+        <v>6266.41</v>
       </c>
       <c r="J12" t="n">
-        <v>7882.3</v>
+        <v>6241.56</v>
       </c>
       <c r="K12" t="n">
-        <v>8253.33</v>
+        <v>6231.55</v>
       </c>
       <c r="L12" t="n">
-        <v>8624.360000000001</v>
+        <v>6227.6</v>
       </c>
       <c r="M12" t="n">
-        <v>8995.389999999999</v>
+        <v>6226.06</v>
       </c>
       <c r="N12" t="n">
-        <v>9366.41</v>
+        <v>6225.46</v>
       </c>
       <c r="O12" t="n">
-        <v>9737.440000000001</v>
+        <v>6225.22</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -879,46 +879,46 @@
         <v>110</v>
       </c>
       <c r="B13" t="n">
-        <v>5196.1</v>
+        <v>5586.86</v>
       </c>
       <c r="C13" t="n">
-        <v>5567.13</v>
+        <v>5258.22</v>
       </c>
       <c r="D13" t="n">
-        <v>5938.16</v>
+        <v>5821.5</v>
       </c>
       <c r="E13" t="n">
-        <v>6309.19</v>
+        <v>6990.73</v>
       </c>
       <c r="F13" t="n">
-        <v>6680.21</v>
+        <v>7093.56</v>
       </c>
       <c r="G13" t="n">
-        <v>7051.24</v>
+        <v>6885.15</v>
       </c>
       <c r="H13" t="n">
-        <v>7422.27</v>
+        <v>6699.09</v>
       </c>
       <c r="I13" t="n">
-        <v>7793.3</v>
+        <v>6597.39</v>
       </c>
       <c r="J13" t="n">
-        <v>8164.33</v>
+        <v>6551.91</v>
       </c>
       <c r="K13" t="n">
-        <v>8535.360000000001</v>
+        <v>6533.2</v>
       </c>
       <c r="L13" t="n">
-        <v>8906.389999999999</v>
+        <v>6525.76</v>
       </c>
       <c r="M13" t="n">
-        <v>9277.41</v>
+        <v>6522.84</v>
       </c>
       <c r="N13" t="n">
-        <v>9648.440000000001</v>
+        <v>6521.71</v>
       </c>
       <c r="O13" t="n">
-        <v>10019.47</v>
+        <v>6521.26</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -926,46 +926,46 @@
         <v>115</v>
       </c>
       <c r="B14" t="n">
-        <v>5478.13</v>
+        <v>5397.08</v>
       </c>
       <c r="C14" t="n">
-        <v>5849.16</v>
+        <v>5144.03</v>
       </c>
       <c r="D14" t="n">
-        <v>6220.18</v>
+        <v>5784.35</v>
       </c>
       <c r="E14" t="n">
-        <v>6591.21</v>
+        <v>7180.28</v>
       </c>
       <c r="F14" t="n">
-        <v>6962.24</v>
+        <v>7447.84</v>
       </c>
       <c r="G14" t="n">
-        <v>7333.27</v>
+        <v>7242.61</v>
       </c>
       <c r="H14" t="n">
-        <v>7704.3</v>
+        <v>6980.58</v>
       </c>
       <c r="I14" t="n">
-        <v>8075.33</v>
+        <v>6814.18</v>
       </c>
       <c r="J14" t="n">
-        <v>8446.360000000001</v>
+        <v>6734.46</v>
       </c>
       <c r="K14" t="n">
-        <v>8817.389999999999</v>
+        <v>6700.7</v>
       </c>
       <c r="L14" t="n">
-        <v>9188.41</v>
+        <v>6687.13</v>
       </c>
       <c r="M14" t="n">
-        <v>9559.440000000001</v>
+        <v>6681.77</v>
       </c>
       <c r="N14" t="n">
-        <v>9930.469999999999</v>
+        <v>6679.68</v>
       </c>
       <c r="O14" t="n">
-        <v>10301.5</v>
+        <v>6678.87</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -973,46 +973,46 @@
         <v>120</v>
       </c>
       <c r="B15" t="n">
-        <v>5760.16</v>
+        <v>5156.67</v>
       </c>
       <c r="C15" t="n">
-        <v>6131.18</v>
+        <v>4974.1</v>
       </c>
       <c r="D15" t="n">
-        <v>6502.21</v>
+        <v>5651.78</v>
       </c>
       <c r="E15" t="n">
-        <v>6873.24</v>
+        <v>7231.12</v>
       </c>
       <c r="F15" t="n">
-        <v>7244.27</v>
+        <v>7685.52</v>
       </c>
       <c r="G15" t="n">
-        <v>7615.3</v>
+        <v>7535.7</v>
       </c>
       <c r="H15" t="n">
-        <v>7986.33</v>
+        <v>7212.02</v>
       </c>
       <c r="I15" t="n">
-        <v>8357.360000000001</v>
+        <v>6962.67</v>
       </c>
       <c r="J15" t="n">
-        <v>8728.389999999999</v>
+        <v>6830.99</v>
       </c>
       <c r="K15" t="n">
-        <v>9099.41</v>
+        <v>6772.73</v>
       </c>
       <c r="L15" t="n">
-        <v>9470.440000000001</v>
+        <v>6748.86</v>
       </c>
       <c r="M15" t="n">
-        <v>9841.469999999999</v>
+        <v>6739.39</v>
       </c>
       <c r="N15" t="n">
-        <v>10212.5</v>
+        <v>6735.67</v>
       </c>
       <c r="O15" t="n">
-        <v>10583.53</v>
+        <v>6734.23</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1020,46 +1020,46 @@
         <v>125</v>
       </c>
       <c r="B16" t="n">
-        <v>6042.18</v>
+        <v>4910.58</v>
       </c>
       <c r="C16" t="n">
-        <v>6413.21</v>
+        <v>4773.46</v>
       </c>
       <c r="D16" t="n">
-        <v>6784.24</v>
+        <v>5456.34</v>
       </c>
       <c r="E16" t="n">
-        <v>7155.27</v>
+        <v>7174.01</v>
       </c>
       <c r="F16" t="n">
-        <v>7526.3</v>
+        <v>7816.02</v>
       </c>
       <c r="G16" t="n">
-        <v>7897.33</v>
+        <v>7769.7</v>
       </c>
       <c r="H16" t="n">
-        <v>8268.360000000001</v>
+        <v>7425.71</v>
       </c>
       <c r="I16" t="n">
-        <v>8639.379999999999</v>
+        <v>7088.39</v>
       </c>
       <c r="J16" t="n">
-        <v>9010.41</v>
+        <v>6884.69</v>
       </c>
       <c r="K16" t="n">
-        <v>9381.440000000001</v>
+        <v>6788.39</v>
       </c>
       <c r="L16" t="n">
-        <v>9752.469999999999</v>
+        <v>6747.78</v>
       </c>
       <c r="M16" t="n">
-        <v>10123.5</v>
+        <v>6731.47</v>
       </c>
       <c r="N16" t="n">
-        <v>10494.53</v>
+        <v>6725.05</v>
       </c>
       <c r="O16" t="n">
-        <v>10865.56</v>
+        <v>6722.54</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1067,46 +1067,46 @@
         <v>130</v>
       </c>
       <c r="B17" t="n">
-        <v>6324.21</v>
+        <v>4674.68</v>
       </c>
       <c r="C17" t="n">
-        <v>6695.24</v>
+        <v>4558.38</v>
       </c>
       <c r="D17" t="n">
-        <v>7066.27</v>
+        <v>5226.06</v>
       </c>
       <c r="E17" t="n">
-        <v>7437.3</v>
+        <v>7041.11</v>
       </c>
       <c r="F17" t="n">
-        <v>7808.33</v>
+        <v>7857.18</v>
       </c>
       <c r="G17" t="n">
-        <v>8179.36</v>
+        <v>7941.18</v>
       </c>
       <c r="H17" t="n">
-        <v>8550.379999999999</v>
+        <v>7631.76</v>
       </c>
       <c r="I17" t="n">
-        <v>8921.41</v>
+        <v>7225.4</v>
       </c>
       <c r="J17" t="n">
-        <v>9292.440000000001</v>
+        <v>6933.3</v>
       </c>
       <c r="K17" t="n">
-        <v>9663.469999999999</v>
+        <v>6781.22</v>
       </c>
       <c r="L17" t="n">
-        <v>10034.5</v>
+        <v>6714.13</v>
       </c>
       <c r="M17" t="n">
-        <v>10405.53</v>
+        <v>6686.67</v>
       </c>
       <c r="N17" t="n">
-        <v>10776.56</v>
+        <v>6675.77</v>
       </c>
       <c r="O17" t="n">
-        <v>11147.58</v>
+        <v>6671.5</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1114,46 +1114,46 @@
         <v>135</v>
       </c>
       <c r="B18" t="n">
-        <v>6606.24</v>
+        <v>4451.65</v>
       </c>
       <c r="C18" t="n">
-        <v>6977.27</v>
+        <v>4340.2</v>
       </c>
       <c r="D18" t="n">
-        <v>7348.3</v>
+        <v>4981.97</v>
       </c>
       <c r="E18" t="n">
-        <v>7719.33</v>
+        <v>6859.15</v>
       </c>
       <c r="F18" t="n">
-        <v>8090.36</v>
+        <v>7830.44</v>
       </c>
       <c r="G18" t="n">
-        <v>8461.379999999999</v>
+        <v>8049.27</v>
       </c>
       <c r="H18" t="n">
-        <v>8832.41</v>
+        <v>7820.62</v>
       </c>
       <c r="I18" t="n">
-        <v>9203.440000000001</v>
+        <v>7388.93</v>
       </c>
       <c r="J18" t="n">
-        <v>9574.469999999999</v>
+        <v>7006.46</v>
       </c>
       <c r="K18" t="n">
-        <v>9945.5</v>
+        <v>6778.93</v>
       </c>
       <c r="L18" t="n">
-        <v>10316.53</v>
+        <v>6671.45</v>
       </c>
       <c r="M18" t="n">
-        <v>10687.56</v>
+        <v>6626.1</v>
       </c>
       <c r="N18" t="n">
-        <v>11058.58</v>
+        <v>6607.87</v>
       </c>
       <c r="O18" t="n">
-        <v>11429.61</v>
+        <v>6600.69</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1161,46 +1161,46 @@
         <v>140</v>
       </c>
       <c r="B19" t="n">
-        <v>6888.27</v>
+        <v>4240.77</v>
       </c>
       <c r="C19" t="n">
-        <v>7259.3</v>
+        <v>4126.83</v>
       </c>
       <c r="D19" t="n">
-        <v>7630.33</v>
+        <v>4738.39</v>
       </c>
       <c r="E19" t="n">
-        <v>8001.36</v>
+        <v>6647.98</v>
       </c>
       <c r="F19" t="n">
-        <v>8372.379999999999</v>
+        <v>7755.78</v>
       </c>
       <c r="G19" t="n">
-        <v>8743.41</v>
+        <v>8100.52</v>
       </c>
       <c r="H19" t="n">
-        <v>9114.440000000001</v>
+        <v>7976.44</v>
       </c>
       <c r="I19" t="n">
-        <v>9485.469999999999</v>
+        <v>7572.67</v>
       </c>
       <c r="J19" t="n">
-        <v>9856.5</v>
+        <v>7122.23</v>
       </c>
       <c r="K19" t="n">
-        <v>10227.53</v>
+        <v>6804.45</v>
       </c>
       <c r="L19" t="n">
-        <v>10598.56</v>
+        <v>6638.59</v>
       </c>
       <c r="M19" t="n">
-        <v>10969.58</v>
+        <v>6565.2</v>
       </c>
       <c r="N19" t="n">
-        <v>11340.61</v>
+        <v>6535.1</v>
       </c>
       <c r="O19" t="n">
-        <v>11711.64</v>
+        <v>6523.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>